<commit_message>
further on the analysis, dataseries analysis left to do
</commit_message>
<xml_diff>
--- a/data/raw_data/neihbourhood_district.xlsx
+++ b/data/raw_data/neihbourhood_district.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lauratll/Documents/Data_Analysis/IronHack/Week_5_Statistics/Project_Week_5/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFAD4A79-16DF-FA40-BEB0-D714631A38D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F107F09-F795-524C-ADA3-43A2905C51C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10760" yWindow="1960" windowWidth="27640" windowHeight="16940" xr2:uid="{63ED238A-0AB7-024B-8EF1-1AC0E594CC81}"/>
   </bookViews>
   <sheets>
     <sheet name="neihbourhood_district" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Neighbourhood</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>F De Aker - Nieuw Sloten</t>
-  </si>
-  <si>
-    <t>K Noord-West</t>
   </si>
   <si>
     <t>K Buitenveldert - Zuidas</t>
@@ -490,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB2741F8-D3BA-1E4E-97FB-E3C7CC8A7584}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="168" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -633,7 +630,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
@@ -646,7 +643,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="5"/>
@@ -659,7 +656,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="5"/>
@@ -672,7 +669,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="5"/>
@@ -683,14 +680,14 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -698,7 +695,7 @@
     </row>
     <row r="16" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -711,7 +708,7 @@
     </row>
     <row r="17" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -724,7 +721,7 @@
     </row>
     <row r="18" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -737,7 +734,7 @@
     </row>
     <row r="19" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -750,7 +747,7 @@
     </row>
     <row r="20" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -763,7 +760,7 @@
     </row>
     <row r="21" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -801,17 +798,9 @@
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="A24" s="1"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -819,19 +808,14 @@
       <c r="E25" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="D27" s="4"/>
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:9" ht="19" x14ac:dyDescent="0.25">
       <c r="E28" s="4"/>
-    </row>
-    <row r="29" spans="1:9" ht="19" x14ac:dyDescent="0.25">
-      <c r="E29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>